<commit_message>
Atualizando o repositório local
</commit_message>
<xml_diff>
--- a/documentação/Product Sprint Backlog.xlsx
+++ b/documentação/Product Sprint Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micazev/paiotnela/documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\paiotnela\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DA1612-E73C-454E-AF96-6EA2000AE462}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4A833B-4AA9-43C6-BBCB-B75F65A6FF51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{1560B7A6-87AF-4E19-B796-FA907A36D599}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1560B7A6-87AF-4E19-B796-FA907A36D599}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -899,7 +899,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,6 +946,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -1114,7 +1121,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1188,46 +1195,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1287,12 +1255,54 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="20% - Ênfase1" xfId="2" builtinId="30"/>
+    <cellStyle name="60% - Ênfase1" xfId="3" builtinId="32"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1314,7 +1324,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1612,21 +1622,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB73C86A-86DA-463D-9718-431C94514CCD}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="65.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1644,7 +1654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1652,11 +1662,11 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1672,9 +1682,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33"/>
-      <c r="B4" s="39" t="s">
+    <row r="4" spans="1:6" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -1690,9 +1700,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
-      <c r="B5" s="39" t="s">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1708,9 +1718,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="57"/>
+      <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1726,9 +1736,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
-      <c r="B7" s="39" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
+      <c r="B7" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1744,9 +1754,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="39" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1762,9 +1772,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="39" t="s">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="57"/>
+      <c r="B9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1780,9 +1790,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
-      <c r="B10" s="39" t="s">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
+      <c r="B10" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1798,9 +1808,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
+      <c r="B11" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1816,9 +1826,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="39" t="s">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="57"/>
+      <c r="B12" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1834,9 +1844,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="39" t="s">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="57"/>
+      <c r="B13" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1852,9 +1862,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="33"/>
-      <c r="B14" s="39" t="s">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="57"/>
+      <c r="B14" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1870,9 +1880,9 @@
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="39" t="s">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
+      <c r="B15" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1888,9 +1898,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="39" t="s">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="57"/>
+      <c r="B16" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1906,9 +1916,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
-      <c r="B17" s="39" t="s">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
+      <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1927,9 +1937,9 @@
         <v>278</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="39" t="s">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="57"/>
+      <c r="B18" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1945,9 +1955,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="33"/>
-      <c r="B19" s="39" t="s">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="57"/>
+      <c r="B19" s="29" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1963,9 +1973,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
-      <c r="B20" s="39" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="57"/>
+      <c r="B20" s="66" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1981,8 +1991,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="33"/>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="57"/>
       <c r="B21" s="10" t="s">
         <v>23</v>
       </c>
@@ -1999,8 +2009,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="33"/>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="57"/>
       <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
@@ -2017,8 +2027,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="33"/>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="57"/>
       <c r="B23" s="10" t="s">
         <v>31</v>
       </c>
@@ -2035,8 +2045,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
       <c r="B24" s="10" t="s">
         <v>40</v>
       </c>
@@ -2053,7 +2063,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="4.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="4.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2061,8 +2071,8 @@
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="58" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -2081,8 +2091,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
       <c r="B27" s="10" t="s">
         <v>45</v>
       </c>
@@ -2099,8 +2109,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="33"/>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="57"/>
       <c r="B28" s="10" t="s">
         <v>46</v>
       </c>
@@ -2117,8 +2127,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
       <c r="B29" s="10" t="s">
         <v>47</v>
       </c>
@@ -2135,8 +2145,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
       <c r="B30" s="10" t="s">
         <v>48</v>
       </c>
@@ -2153,7 +2163,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="3.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2161,8 +2171,8 @@
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:7" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+    <row r="32" spans="1:7" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -2181,8 +2191,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
       <c r="B33" s="10" t="s">
         <v>44</v>
       </c>
@@ -2199,8 +2209,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
       <c r="B34" s="10" t="s">
         <v>45</v>
       </c>
@@ -2217,8 +2227,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
       <c r="B35" s="10" t="s">
         <v>46</v>
       </c>
@@ -2235,8 +2245,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
       <c r="B36" s="10" t="s">
         <v>47</v>
       </c>
@@ -2253,8 +2263,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="54"/>
       <c r="B37" s="10" t="s">
         <v>48</v>
       </c>
@@ -2271,8 +2281,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="55"/>
       <c r="B38" s="10" t="s">
         <v>66</v>
       </c>
@@ -2289,7 +2299,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="3.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2297,8 +2307,8 @@
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="56" t="s">
         <v>68</v>
       </c>
       <c r="B40" s="10" t="s">
@@ -2317,8 +2327,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="33"/>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="57"/>
       <c r="B41" s="10" t="s">
         <v>5</v>
       </c>
@@ -2335,8 +2345,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="33"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="57"/>
       <c r="B42" s="10" t="s">
         <v>6</v>
       </c>
@@ -2353,8 +2363,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="33"/>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="57"/>
       <c r="B43" s="10" t="s">
         <v>7</v>
       </c>
@@ -2371,8 +2381,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="33"/>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="57"/>
       <c r="B44" s="10" t="s">
         <v>44</v>
       </c>
@@ -2389,8 +2399,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A45" s="33"/>
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="57"/>
       <c r="B45" s="10" t="s">
         <v>45</v>
       </c>
@@ -2407,7 +2417,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="4.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2415,8 +2425,8 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
+    <row r="47" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="53" t="s">
         <v>85</v>
       </c>
       <c r="B47" s="12" t="s">
@@ -2435,8 +2445,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="30"/>
+    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
       <c r="B48" s="26" t="s">
         <v>4</v>
       </c>
@@ -2453,8 +2463,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="30"/>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
       <c r="B49" s="26" t="s">
         <v>5</v>
       </c>
@@ -2471,8 +2481,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="30"/>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="54"/>
       <c r="B50" s="26" t="s">
         <v>6</v>
       </c>
@@ -2489,8 +2499,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="30"/>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="54"/>
       <c r="B51" s="26" t="s">
         <v>7</v>
       </c>
@@ -2507,8 +2517,8 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" s="30"/>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="54"/>
       <c r="B52" s="26" t="s">
         <v>8</v>
       </c>
@@ -2525,8 +2535,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="54"/>
       <c r="B53" s="26" t="s">
         <v>9</v>
       </c>
@@ -2543,8 +2553,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="31"/>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="55"/>
       <c r="B54" s="26" t="s">
         <v>10</v>
       </c>
@@ -2598,32 +2608,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5994EBB2-7D56-4B66-AE3B-20C2BD3DC2FB}">
   <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0.6640625" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="0.7109375" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E1" s="45" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E1" s="32" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="62"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="6" t="s">
         <v>87</v>
       </c>
@@ -2637,27 +2647,27 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="3.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="58"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="33">
         <v>2</v>
       </c>
       <c r="F4" s="17" t="s">
@@ -2665,14 +2675,14 @@
       </c>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="58"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="47"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="33">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
@@ -2680,14 +2690,14 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="58"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="33">
         <v>1</v>
       </c>
       <c r="F6" s="17" t="s">
@@ -2695,16 +2705,16 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
-      <c r="B7" s="40" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="44" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="42">
         <v>1</v>
       </c>
       <c r="F7" s="17" t="s">
@@ -2712,14 +2722,14 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="44" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="42">
         <v>1</v>
       </c>
       <c r="F8" s="17" t="s">
@@ -2727,14 +2737,14 @@
       </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="60"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="44" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="42">
         <v>1</v>
       </c>
       <c r="F9" s="17" t="s">
@@ -2742,14 +2752,14 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="44" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="42">
         <v>1</v>
       </c>
       <c r="F10" s="17" t="s">
@@ -2757,16 +2767,16 @@
       </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="60"/>
-      <c r="B11" s="40" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="33">
         <v>1</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -2774,14 +2784,14 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="60"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="58"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="33">
         <v>2</v>
       </c>
       <c r="F12" s="17" t="s">
@@ -2789,14 +2799,14 @@
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="60"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="58"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="33">
         <v>1</v>
       </c>
       <c r="F13" s="17" t="s">
@@ -2804,14 +2814,14 @@
       </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="58"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="33">
         <v>2</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -2819,16 +2829,16 @@
       </c>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="40" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="44" t="s">
+      <c r="C15" s="45"/>
+      <c r="D15" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="E15" s="55">
+      <c r="E15" s="42">
         <v>1</v>
       </c>
       <c r="F15" s="17" t="s">
@@ -2836,14 +2846,14 @@
       </c>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="44" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="E16" s="55">
+      <c r="E16" s="42">
         <v>2</v>
       </c>
       <c r="F16" s="17" t="s">
@@ -2851,14 +2861,14 @@
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="60"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="44" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="E17" s="55">
+      <c r="E17" s="42">
         <v>1</v>
       </c>
       <c r="F17" s="17" t="s">
@@ -2866,14 +2876,14 @@
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="44" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="E18" s="55">
+      <c r="E18" s="42">
         <v>2</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -2881,16 +2891,16 @@
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="60"/>
-      <c r="B19" s="49" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="33">
         <v>1</v>
       </c>
       <c r="F19" s="17" t="s">
@@ -2898,14 +2908,14 @@
       </c>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="60"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="58"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="46">
+      <c r="E20" s="33">
         <v>1</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -2913,14 +2923,14 @@
       </c>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="58"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="33">
         <v>2</v>
       </c>
       <c r="F21" s="17" t="s">
@@ -2928,16 +2938,16 @@
       </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="40" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="B22" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="44" t="s">
+      <c r="C22" s="45"/>
+      <c r="D22" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="E22" s="55">
+      <c r="E22" s="42">
         <v>1</v>
       </c>
       <c r="F22" s="17" t="s">
@@ -2945,14 +2955,14 @@
       </c>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="44" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="55">
+      <c r="E23" s="42">
         <v>1</v>
       </c>
       <c r="F23" s="17" t="s">
@@ -2960,14 +2970,14 @@
       </c>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="44" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="E24" s="55">
+      <c r="E24" s="42">
         <v>1</v>
       </c>
       <c r="F24" s="17" t="s">
@@ -2975,14 +2985,14 @@
       </c>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="44" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="47"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="E25" s="55">
+      <c r="E25" s="42">
         <v>2</v>
       </c>
       <c r="F25" s="17" t="s">
@@ -2990,16 +3000,16 @@
       </c>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
-      <c r="B26" s="40" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="B26" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="58"/>
+      <c r="C26" s="45"/>
       <c r="D26" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="46">
+      <c r="E26" s="33">
         <v>1</v>
       </c>
       <c r="F26" s="17" t="s">
@@ -3007,14 +3017,14 @@
       </c>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="58"/>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="47"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="45"/>
       <c r="D27" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="E27" s="46">
+      <c r="E27" s="33">
         <v>2</v>
       </c>
       <c r="F27" s="17" t="s">
@@ -3022,14 +3032,14 @@
       </c>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="58"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="E28" s="46">
+      <c r="E28" s="33">
         <v>1</v>
       </c>
       <c r="F28" s="17" t="s">
@@ -3037,16 +3047,16 @@
       </c>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
-      <c r="B29" s="40" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="47"/>
+      <c r="B29" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="58"/>
-      <c r="D29" s="44" t="s">
+      <c r="C29" s="45"/>
+      <c r="D29" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="E29" s="55">
+      <c r="E29" s="42">
         <v>1</v>
       </c>
       <c r="F29" s="17" t="s">
@@ -3054,14 +3064,14 @@
       </c>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="44" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="E30" s="55">
+      <c r="E30" s="42">
         <v>1</v>
       </c>
       <c r="F30" s="17" t="s">
@@ -3069,16 +3079,16 @@
       </c>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
-      <c r="B31" s="40" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="E31" s="46">
+      <c r="E31" s="33">
         <v>1</v>
       </c>
       <c r="F31" s="17" t="s">
@@ -3086,14 +3096,14 @@
       </c>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="58"/>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="E32" s="46">
+      <c r="E32" s="33">
         <v>1</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -3101,14 +3111,14 @@
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="60"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="58"/>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E33" s="46">
+      <c r="E33" s="33">
         <v>1</v>
       </c>
       <c r="F33" s="17" t="s">
@@ -3116,14 +3126,14 @@
       </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="58"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="45"/>
       <c r="D34" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="E34" s="46">
+      <c r="E34" s="33">
         <v>1</v>
       </c>
       <c r="F34" s="17" t="s">
@@ -3131,14 +3141,14 @@
       </c>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="58"/>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="E35" s="46">
+      <c r="E35" s="33">
         <v>1</v>
       </c>
       <c r="F35" s="17" t="s">
@@ -3146,14 +3156,14 @@
       </c>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="58"/>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="45"/>
       <c r="D36" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="E36" s="46">
+      <c r="E36" s="33">
         <v>1</v>
       </c>
       <c r="F36" s="17" t="s">
@@ -3161,14 +3171,14 @@
       </c>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="58"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="E37" s="46">
+      <c r="E37" s="33">
         <v>1</v>
       </c>
       <c r="F37" s="17" t="s">
@@ -3176,14 +3186,14 @@
       </c>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="60"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="58"/>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="45"/>
       <c r="D38" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="E38" s="46">
+      <c r="E38" s="33">
         <v>1</v>
       </c>
       <c r="F38" s="17" t="s">
@@ -3191,14 +3201,14 @@
       </c>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="60"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="58"/>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="45"/>
       <c r="D39" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="E39" s="46">
+      <c r="E39" s="33">
         <v>1</v>
       </c>
       <c r="F39" s="17" t="s">
@@ -3206,14 +3216,14 @@
       </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="58"/>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="45"/>
       <c r="D40" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="E40" s="46">
+      <c r="E40" s="33">
         <v>1</v>
       </c>
       <c r="F40" s="17" t="s">
@@ -3221,14 +3231,14 @@
       </c>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="58"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="45"/>
       <c r="D41" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="E41" s="46">
+      <c r="E41" s="33">
         <v>1</v>
       </c>
       <c r="F41" s="17" t="s">
@@ -3236,14 +3246,14 @@
       </c>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="58"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="45"/>
       <c r="D42" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="E42" s="46">
+      <c r="E42" s="33">
         <v>1</v>
       </c>
       <c r="F42" s="17" t="s">
@@ -3251,14 +3261,14 @@
       </c>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="60"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="58"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="E43" s="46">
+      <c r="E43" s="33">
         <v>1</v>
       </c>
       <c r="F43" s="17" t="s">
@@ -3266,14 +3276,14 @@
       </c>
       <c r="G43" s="14"/>
     </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="58"/>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="47"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="E44" s="46">
+      <c r="E44" s="33">
         <v>1</v>
       </c>
       <c r="F44" s="17" t="s">
@@ -3281,14 +3291,14 @@
       </c>
       <c r="G44" s="14"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="58"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="47"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="45"/>
       <c r="D45" t="s">
         <v>257</v>
       </c>
-      <c r="E45" s="46">
+      <c r="E45" s="33">
         <v>1</v>
       </c>
       <c r="F45" s="17" t="s">
@@ -3296,14 +3306,14 @@
       </c>
       <c r="G45" s="14"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="58"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="47"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="45"/>
       <c r="D46" t="s">
         <v>258</v>
       </c>
-      <c r="E46" s="46">
+      <c r="E46" s="33">
         <v>1</v>
       </c>
       <c r="F46" s="17" t="s">
@@ -3311,14 +3321,14 @@
       </c>
       <c r="G46" s="14"/>
     </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="58"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="47"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="45"/>
       <c r="D47" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="E47" s="46">
+      <c r="E47" s="33">
         <v>3</v>
       </c>
       <c r="F47" s="17" t="s">
@@ -3326,16 +3336,16 @@
       </c>
       <c r="G47" s="14"/>
     </row>
-    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="40" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="47"/>
+      <c r="B48" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="44" t="s">
+      <c r="C48" s="45"/>
+      <c r="D48" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="E48" s="55">
+      <c r="E48" s="42">
         <v>2</v>
       </c>
       <c r="F48" s="17" t="s">
@@ -3343,14 +3353,14 @@
       </c>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="44" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="47"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="E49" s="55">
+      <c r="E49" s="42">
         <v>2</v>
       </c>
       <c r="F49" s="17" t="s">
@@ -3358,14 +3368,14 @@
       </c>
       <c r="G49" s="14"/>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="44" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="47"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="E50" s="55">
+      <c r="E50" s="42">
         <v>2</v>
       </c>
       <c r="F50" s="17" t="s">
@@ -3373,16 +3383,16 @@
       </c>
       <c r="G50" s="14"/>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="40" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="47"/>
+      <c r="B51" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="56" t="s">
+      <c r="C51" s="45"/>
+      <c r="D51" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="E51" s="46">
+      <c r="E51" s="33">
         <v>2</v>
       </c>
       <c r="F51" s="17" t="s">
@@ -3390,14 +3400,14 @@
       </c>
       <c r="G51" s="14"/>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="56" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="47"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="E52" s="46">
+      <c r="E52" s="33">
         <v>2</v>
       </c>
       <c r="F52" s="17" t="s">
@@ -3405,14 +3415,14 @@
       </c>
       <c r="G52" s="14"/>
     </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="42"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="56" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="47"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="E53" s="46">
+      <c r="E53" s="33">
         <v>1</v>
       </c>
       <c r="F53" s="17" t="s">
@@ -3420,16 +3430,16 @@
       </c>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="40" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="47"/>
+      <c r="B54" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="58"/>
-      <c r="D54" s="44" t="s">
+      <c r="C54" s="45"/>
+      <c r="D54" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="E54" s="57">
+      <c r="E54" s="44">
         <v>1</v>
       </c>
       <c r="F54" s="17" t="s">
@@ -3437,14 +3447,14 @@
       </c>
       <c r="G54" s="14"/>
     </row>
-    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="41"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="44" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="47"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="E55" s="57">
+      <c r="E55" s="44">
         <v>1</v>
       </c>
       <c r="F55" s="17" t="s">
@@ -3452,14 +3462,14 @@
       </c>
       <c r="G55" s="14"/>
     </row>
-    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="60"/>
-      <c r="B56" s="42"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="44" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="47"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="E56" s="57">
+      <c r="E56" s="44">
         <v>1</v>
       </c>
       <c r="F56" s="17" t="s">
@@ -3467,16 +3477,16 @@
       </c>
       <c r="G56" s="14"/>
     </row>
-    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="60"/>
-      <c r="B57" s="40" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="47"/>
+      <c r="B57" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="58"/>
-      <c r="D57" s="44" t="s">
+      <c r="C57" s="45"/>
+      <c r="D57" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E57" s="57">
+      <c r="E57" s="44">
         <v>1</v>
       </c>
       <c r="F57" s="17" t="s">
@@ -3484,14 +3494,14 @@
       </c>
       <c r="G57" s="14"/>
     </row>
-    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="60"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="44" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="47"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="E58" s="57">
+      <c r="E58" s="44">
         <v>1</v>
       </c>
       <c r="F58" s="17" t="s">
@@ -3499,16 +3509,16 @@
       </c>
       <c r="G58" s="14"/>
     </row>
-    <row r="59" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A59" s="60"/>
-      <c r="B59" s="40" t="s">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="47"/>
+      <c r="B59" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="58"/>
+      <c r="C59" s="45"/>
       <c r="D59" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="E59" s="46">
+      <c r="E59" s="33">
         <v>14</v>
       </c>
       <c r="F59" s="18" t="s">
@@ -3516,14 +3526,14 @@
       </c>
       <c r="G59" s="14"/>
     </row>
-    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="60"/>
-      <c r="B60" s="41"/>
-      <c r="C60" s="58"/>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="47"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="45"/>
       <c r="D60" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="E60" s="46">
+      <c r="E60" s="33">
         <v>1</v>
       </c>
       <c r="F60" s="17" t="s">
@@ -3531,14 +3541,14 @@
       </c>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A61" s="60"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="58"/>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="47"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="45"/>
       <c r="D61" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="E61" s="48">
+      <c r="E61" s="35">
         <v>14</v>
       </c>
       <c r="F61" s="18" t="s">
@@ -3546,53 +3556,53 @@
       </c>
       <c r="G61" s="14"/>
     </row>
-    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="60"/>
-      <c r="B62" s="40" t="s">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="47"/>
+      <c r="B62" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="58"/>
-      <c r="D62" s="44" t="s">
+      <c r="C62" s="45"/>
+      <c r="D62" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E62" s="43"/>
+      <c r="E62" s="30"/>
       <c r="F62" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G62" s="14"/>
     </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="60"/>
-      <c r="B63" s="41"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="44" t="s">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="47"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="45"/>
+      <c r="D63" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E63" s="43"/>
+      <c r="E63" s="30"/>
       <c r="F63" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G63" s="14"/>
     </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="60"/>
-      <c r="B64" s="42"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="44" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="47"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="E64" s="43"/>
+      <c r="E64" s="30"/>
       <c r="F64" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G64" s="14"/>
     </row>
-    <row r="65" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A65" s="60"/>
-      <c r="B65" s="40" t="s">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="47"/>
+      <c r="B65" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="58"/>
+      <c r="C65" s="45"/>
       <c r="D65" s="20" t="s">
         <v>98</v>
       </c>
@@ -3602,10 +3612,10 @@
       </c>
       <c r="G65" s="14"/>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="60"/>
-      <c r="B66" s="41"/>
-      <c r="C66" s="58"/>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="47"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="45"/>
       <c r="D66" s="20" t="s">
         <v>99</v>
       </c>
@@ -3615,10 +3625,10 @@
       </c>
       <c r="G66" s="14"/>
     </row>
-    <row r="67" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A67" s="60"/>
-      <c r="B67" s="42"/>
-      <c r="C67" s="58"/>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="47"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="45"/>
       <c r="D67" s="20" t="s">
         <v>101</v>
       </c>
@@ -3630,53 +3640,53 @@
       </c>
       <c r="G67" s="14"/>
     </row>
-    <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A68" s="60"/>
-      <c r="B68" s="40" t="s">
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="47"/>
+      <c r="B68" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="58"/>
-      <c r="D68" s="44" t="s">
+      <c r="C68" s="45"/>
+      <c r="D68" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E68" s="43"/>
+      <c r="E68" s="30"/>
       <c r="F68" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G68" s="14"/>
     </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="60"/>
-      <c r="B69" s="41"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="44" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="47"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E69" s="43"/>
+      <c r="E69" s="30"/>
       <c r="F69" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G69" s="14"/>
     </row>
-    <row r="70" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A70" s="61"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="44" t="s">
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="48"/>
+      <c r="B70" s="61"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E70" s="43"/>
+      <c r="E70" s="30"/>
       <c r="F70" s="19" t="s">
         <v>279</v>
       </c>
       <c r="G70" s="14"/>
     </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
-      <c r="B71" s="40" t="s">
+      <c r="B71" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C71" s="58"/>
+      <c r="C71" s="45"/>
       <c r="D71" s="20" t="s">
         <v>105</v>
       </c>
@@ -3686,10 +3696,10 @@
       </c>
       <c r="G71" s="14"/>
     </row>
-    <row r="72" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="59"/>
-      <c r="B72" s="41"/>
-      <c r="C72" s="58"/>
+    <row r="72" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="46"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="45"/>
       <c r="D72" s="20" t="s">
         <v>106</v>
       </c>
@@ -3699,10 +3709,10 @@
       </c>
       <c r="G72" s="14"/>
     </row>
-    <row r="73" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A73" s="60"/>
-      <c r="B73" s="42"/>
-      <c r="C73" s="58"/>
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="47"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="45"/>
       <c r="D73" s="20" t="s">
         <v>107</v>
       </c>
@@ -3712,53 +3722,53 @@
       </c>
       <c r="G73" s="14"/>
     </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="60"/>
-      <c r="B74" s="35" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="47"/>
+      <c r="B74" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="58"/>
-      <c r="D74" s="44" t="s">
+      <c r="C74" s="45"/>
+      <c r="D74" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E74" s="43"/>
+      <c r="E74" s="30"/>
       <c r="F74" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G74" s="14"/>
     </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="60"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="44" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="47"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="45"/>
+      <c r="D75" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E75" s="43"/>
+      <c r="E75" s="30"/>
       <c r="F75" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="60"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="44" t="s">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="47"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="45"/>
+      <c r="D76" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="E76" s="43"/>
+      <c r="E76" s="30"/>
       <c r="F76" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G76" s="14"/>
     </row>
-    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="60"/>
-      <c r="B77" s="35" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="47"/>
+      <c r="B77" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C77" s="58"/>
+      <c r="C77" s="45"/>
       <c r="D77" s="20" t="s">
         <v>111</v>
       </c>
@@ -3768,10 +3778,10 @@
       </c>
       <c r="G77" s="14"/>
     </row>
-    <row r="78" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A78" s="60"/>
-      <c r="B78" s="36"/>
-      <c r="C78" s="58"/>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="47"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="45"/>
       <c r="D78" s="20" t="s">
         <v>112</v>
       </c>
@@ -3781,10 +3791,10 @@
       </c>
       <c r="G78" s="14"/>
     </row>
-    <row r="79" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A79" s="60"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="58"/>
+    <row r="79" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="47"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="45"/>
       <c r="D79" s="20" t="s">
         <v>113</v>
       </c>
@@ -3796,16 +3806,16 @@
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A80" s="60"/>
-      <c r="B80" s="35" t="s">
+    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="47"/>
+      <c r="B80" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C80" s="58"/>
-      <c r="D80" s="44" t="s">
+      <c r="C80" s="45"/>
+      <c r="D80" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="E80" s="43"/>
+      <c r="E80" s="30"/>
       <c r="F80" s="17" t="s">
         <v>172</v>
       </c>
@@ -3813,38 +3823,38 @@
         <v>175</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A81" s="60"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="44" t="s">
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="47"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="E81" s="43"/>
+      <c r="E81" s="30"/>
       <c r="F81" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G81" s="14"/>
     </row>
-    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="60"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="44" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="47"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E82" s="43"/>
+      <c r="E82" s="30"/>
       <c r="F82" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G82" s="14"/>
     </row>
-    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="60"/>
-      <c r="B83" s="35" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="47"/>
+      <c r="B83" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C83" s="58"/>
+      <c r="C83" s="45"/>
       <c r="D83" s="20" t="s">
         <v>117</v>
       </c>
@@ -3854,10 +3864,10 @@
       </c>
       <c r="G83" s="14"/>
     </row>
-    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="60"/>
-      <c r="B84" s="36"/>
-      <c r="C84" s="58"/>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="47"/>
+      <c r="B84" s="63"/>
+      <c r="C84" s="45"/>
       <c r="D84" s="20" t="s">
         <v>118</v>
       </c>
@@ -3867,10 +3877,10 @@
       </c>
       <c r="G84" s="14"/>
     </row>
-    <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="61"/>
-      <c r="B85" s="37"/>
-      <c r="C85" s="58"/>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="48"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="45"/>
       <c r="D85" s="20" t="s">
         <v>119</v>
       </c>
@@ -3880,654 +3890,653 @@
       </c>
       <c r="G85" s="14"/>
     </row>
-    <row r="86" spans="1:7" ht="2.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="58"/>
+      <c r="B86" s="62"/>
+      <c r="C86" s="45"/>
       <c r="D86" s="20"/>
       <c r="E86" s="4"/>
       <c r="F86" s="3"/>
       <c r="G86" s="14"/>
     </row>
-    <row r="87" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="59"/>
-      <c r="B87" s="36"/>
-      <c r="C87" s="58"/>
+    <row r="87" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="46"/>
+      <c r="B87" s="63"/>
+      <c r="C87" s="45"/>
       <c r="D87" s="20"/>
-      <c r="E87" s="46"/>
+      <c r="E87" s="33"/>
       <c r="F87" s="17"/>
       <c r="G87" s="14"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="60"/>
-      <c r="B88" s="37"/>
-      <c r="C88" s="58"/>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="47"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="45"/>
       <c r="D88" s="16"/>
-      <c r="E88" s="46"/>
+      <c r="E88" s="33"/>
       <c r="F88" s="17"/>
       <c r="G88" s="14"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="60"/>
-      <c r="B89" s="53"/>
-      <c r="C89" s="58"/>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="47"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="45"/>
       <c r="D89" s="20"/>
-      <c r="E89" s="46"/>
+      <c r="E89" s="33"/>
       <c r="F89" s="17"/>
       <c r="G89" s="14"/>
     </row>
-    <row r="90" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="60"/>
-      <c r="B90" s="54"/>
-      <c r="C90" s="58"/>
+    <row r="90" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="47"/>
+      <c r="B90" s="41"/>
+      <c r="C90" s="45"/>
       <c r="D90" s="20"/>
-      <c r="E90" s="46"/>
+      <c r="E90" s="33"/>
       <c r="F90" s="17"/>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="60"/>
-      <c r="B91" s="52"/>
-      <c r="C91" s="58"/>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="47"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="45"/>
       <c r="D91" s="20"/>
-      <c r="E91" s="46"/>
+      <c r="E91" s="33"/>
       <c r="F91" s="19"/>
       <c r="G91" s="14"/>
     </row>
-    <row r="92" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="60"/>
-      <c r="B92" s="53"/>
-      <c r="C92" s="58"/>
+    <row r="92" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="47"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="45"/>
       <c r="D92" s="20"/>
-      <c r="E92" s="46"/>
+      <c r="E92" s="33"/>
       <c r="F92" s="19"/>
       <c r="G92" s="14"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="60"/>
-      <c r="B93" s="54"/>
-      <c r="C93" s="58"/>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="47"/>
+      <c r="B93" s="41"/>
+      <c r="C93" s="45"/>
       <c r="D93" s="20"/>
-      <c r="E93" s="46"/>
+      <c r="E93" s="33"/>
       <c r="F93" s="19"/>
       <c r="G93" s="14"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="60"/>
-      <c r="B94" s="52"/>
-      <c r="C94" s="58"/>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="47"/>
+      <c r="B94" s="39"/>
+      <c r="C94" s="45"/>
       <c r="D94" s="20"/>
-      <c r="E94" s="46"/>
+      <c r="E94" s="33"/>
       <c r="F94" s="19"/>
       <c r="G94" s="14"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="60"/>
-      <c r="B95" s="53"/>
-      <c r="C95" s="58"/>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="47"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="45"/>
       <c r="D95" s="20"/>
-      <c r="E95" s="46"/>
+      <c r="E95" s="33"/>
       <c r="F95" s="19"/>
       <c r="G95" s="14"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="60"/>
-      <c r="B96" s="53"/>
-      <c r="C96" s="58"/>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="47"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="45"/>
       <c r="D96" s="20"/>
-      <c r="E96" s="46"/>
+      <c r="E96" s="33"/>
       <c r="F96" s="19"/>
       <c r="G96" s="14"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="60"/>
-      <c r="B97" s="54"/>
-      <c r="C97" s="58"/>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="47"/>
+      <c r="B97" s="41"/>
+      <c r="C97" s="45"/>
       <c r="D97" s="20"/>
-      <c r="E97" s="46"/>
+      <c r="E97" s="33"/>
       <c r="F97" s="19"/>
       <c r="G97" s="14"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="60"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="58"/>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="47"/>
+      <c r="B98" s="39"/>
+      <c r="C98" s="45"/>
       <c r="D98" s="20"/>
-      <c r="E98" s="46"/>
+      <c r="E98" s="33"/>
       <c r="F98" s="19"/>
       <c r="G98" s="14"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="60"/>
-      <c r="B99" s="53"/>
-      <c r="C99" s="58"/>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="47"/>
+      <c r="B99" s="40"/>
+      <c r="C99" s="45"/>
       <c r="D99" s="20"/>
-      <c r="E99" s="46"/>
+      <c r="E99" s="33"/>
       <c r="F99" s="19"/>
       <c r="G99" s="14"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="60"/>
-      <c r="B100" s="54"/>
-      <c r="C100" s="58"/>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="47"/>
+      <c r="B100" s="41"/>
+      <c r="C100" s="45"/>
       <c r="D100" s="20"/>
-      <c r="E100" s="46"/>
+      <c r="E100" s="33"/>
       <c r="F100" s="19"/>
       <c r="G100" s="14"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="60"/>
-      <c r="B101" s="52"/>
-      <c r="C101" s="58"/>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="47"/>
+      <c r="B101" s="39"/>
+      <c r="C101" s="45"/>
       <c r="D101" s="20"/>
-      <c r="E101" s="46"/>
+      <c r="E101" s="33"/>
       <c r="F101" s="19"/>
       <c r="G101" s="14"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="60"/>
-      <c r="B102" s="53"/>
-      <c r="C102" s="58"/>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="47"/>
+      <c r="B102" s="40"/>
+      <c r="C102" s="45"/>
       <c r="D102" s="20"/>
-      <c r="E102" s="46"/>
+      <c r="E102" s="33"/>
       <c r="F102" s="19"/>
       <c r="G102" s="14"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="60"/>
-      <c r="B103" s="54"/>
-      <c r="C103" s="58"/>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="47"/>
+      <c r="B103" s="41"/>
+      <c r="C103" s="45"/>
       <c r="D103" s="20"/>
-      <c r="E103" s="46"/>
+      <c r="E103" s="33"/>
       <c r="F103" s="19"/>
       <c r="G103" s="14"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="60"/>
-      <c r="B104" s="52"/>
-      <c r="C104" s="58"/>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="47"/>
+      <c r="B104" s="39"/>
+      <c r="C104" s="45"/>
       <c r="D104" s="20"/>
-      <c r="E104" s="46"/>
+      <c r="E104" s="33"/>
       <c r="F104" s="19"/>
       <c r="G104" s="14"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="60"/>
-      <c r="B105" s="53"/>
-      <c r="C105" s="58"/>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="47"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="45"/>
       <c r="D105" s="20"/>
-      <c r="E105" s="46"/>
+      <c r="E105" s="33"/>
       <c r="F105" s="19"/>
       <c r="G105" s="14"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="60"/>
-      <c r="B106" s="54"/>
-      <c r="C106" s="58"/>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="47"/>
+      <c r="B106" s="41"/>
+      <c r="C106" s="45"/>
       <c r="D106" s="20"/>
-      <c r="E106" s="46"/>
+      <c r="E106" s="33"/>
       <c r="F106" s="19"/>
       <c r="G106" s="14"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="60"/>
-      <c r="B107" s="52"/>
-      <c r="C107" s="58"/>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="47"/>
+      <c r="B107" s="39"/>
+      <c r="C107" s="45"/>
       <c r="D107" s="20"/>
-      <c r="E107" s="46"/>
+      <c r="E107" s="33"/>
       <c r="F107" s="19"/>
       <c r="G107" s="14"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="60"/>
-      <c r="B108" s="53"/>
-      <c r="C108" s="58"/>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="47"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="45"/>
       <c r="D108" s="20"/>
-      <c r="E108" s="46"/>
+      <c r="E108" s="33"/>
       <c r="F108" s="19"/>
       <c r="G108" s="14"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="61"/>
-      <c r="B109" s="54"/>
-      <c r="C109" s="58"/>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="48"/>
+      <c r="B109" s="41"/>
+      <c r="C109" s="45"/>
       <c r="D109" s="20"/>
-      <c r="E109" s="46"/>
+      <c r="E109" s="33"/>
       <c r="F109" s="19"/>
       <c r="G109" s="14"/>
     </row>
-    <row r="110" spans="1:7" ht="2.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
-      <c r="C110" s="58"/>
+      <c r="C110" s="45"/>
       <c r="D110" s="20"/>
       <c r="E110" s="4"/>
       <c r="F110" s="3"/>
       <c r="G110" s="14"/>
     </row>
-    <row r="111" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="59"/>
-      <c r="B111" s="52"/>
-      <c r="C111" s="58"/>
+    <row r="111" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="46"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="45"/>
       <c r="D111" s="20"/>
-      <c r="E111" s="46"/>
+      <c r="E111" s="33"/>
       <c r="F111" s="17"/>
       <c r="G111" s="14"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="60"/>
-      <c r="B112" s="53"/>
-      <c r="C112" s="58"/>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="47"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="45"/>
       <c r="D112" s="21"/>
-      <c r="E112" s="46"/>
+      <c r="E112" s="33"/>
       <c r="F112" s="17"/>
       <c r="G112" s="14"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="60"/>
-      <c r="B113" s="54"/>
-      <c r="C113" s="58"/>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="47"/>
+      <c r="B113" s="41"/>
+      <c r="C113" s="45"/>
       <c r="D113" s="20"/>
-      <c r="E113" s="46"/>
+      <c r="E113" s="33"/>
       <c r="F113" s="17"/>
       <c r="G113" s="14"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="60"/>
-      <c r="B114" s="52"/>
-      <c r="C114" s="58"/>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="47"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="45"/>
       <c r="D114" s="20"/>
-      <c r="E114" s="46"/>
+      <c r="E114" s="33"/>
       <c r="F114" s="19"/>
       <c r="G114" s="3"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="60"/>
-      <c r="B115" s="53"/>
-      <c r="C115" s="58"/>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="47"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="45"/>
       <c r="D115" s="20"/>
-      <c r="E115" s="46"/>
+      <c r="E115" s="33"/>
       <c r="F115" s="19"/>
       <c r="G115" s="14"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="60"/>
-      <c r="B116" s="54"/>
-      <c r="C116" s="58"/>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="47"/>
+      <c r="B116" s="41"/>
+      <c r="C116" s="45"/>
       <c r="D116" s="20"/>
-      <c r="E116" s="46"/>
+      <c r="E116" s="33"/>
       <c r="F116" s="19"/>
       <c r="G116" s="14"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="60"/>
-      <c r="B117" s="52"/>
-      <c r="C117" s="58"/>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="47"/>
+      <c r="B117" s="39"/>
+      <c r="C117" s="45"/>
       <c r="D117" s="20"/>
-      <c r="E117" s="46"/>
+      <c r="E117" s="33"/>
       <c r="F117" s="17"/>
       <c r="G117" s="14"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="60"/>
-      <c r="B118" s="53"/>
-      <c r="C118" s="58"/>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="47"/>
+      <c r="B118" s="40"/>
+      <c r="C118" s="45"/>
       <c r="D118" s="20"/>
-      <c r="E118" s="46"/>
+      <c r="E118" s="33"/>
       <c r="F118" s="17"/>
       <c r="G118" s="14"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="60"/>
-      <c r="B119" s="54"/>
-      <c r="C119" s="58"/>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="47"/>
+      <c r="B119" s="41"/>
+      <c r="C119" s="45"/>
       <c r="D119" s="20"/>
-      <c r="E119" s="46"/>
+      <c r="E119" s="33"/>
       <c r="F119" s="17"/>
       <c r="G119" s="14"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="60"/>
-      <c r="B120" s="52"/>
-      <c r="C120" s="58"/>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="47"/>
+      <c r="B120" s="39"/>
+      <c r="C120" s="45"/>
       <c r="D120" s="20"/>
-      <c r="E120" s="46"/>
+      <c r="E120" s="33"/>
       <c r="F120" s="18"/>
       <c r="G120" s="14"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="60"/>
-      <c r="B121" s="53"/>
-      <c r="C121" s="58"/>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="47"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="45"/>
       <c r="D121" s="20"/>
-      <c r="E121" s="46"/>
+      <c r="E121" s="33"/>
       <c r="F121" s="18"/>
       <c r="G121" s="14"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="60"/>
-      <c r="B122" s="54"/>
-      <c r="C122" s="58"/>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="47"/>
+      <c r="B122" s="41"/>
+      <c r="C122" s="45"/>
       <c r="D122" s="20"/>
-      <c r="E122" s="46"/>
+      <c r="E122" s="33"/>
       <c r="F122" s="18"/>
       <c r="G122" s="14"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="60"/>
-      <c r="B123" s="52"/>
-      <c r="C123" s="58"/>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="47"/>
+      <c r="B123" s="39"/>
+      <c r="C123" s="45"/>
       <c r="D123" s="20"/>
-      <c r="E123" s="46"/>
+      <c r="E123" s="33"/>
       <c r="F123" s="17"/>
       <c r="G123" s="14"/>
     </row>
-    <row r="124" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A124" s="60"/>
-      <c r="B124" s="53"/>
-      <c r="C124" s="58"/>
+    <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A124" s="47"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="45"/>
       <c r="D124" s="20"/>
-      <c r="E124" s="46"/>
+      <c r="E124" s="33"/>
       <c r="F124" s="17"/>
       <c r="G124" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A125" s="60"/>
-      <c r="B125" s="54"/>
-      <c r="C125" s="58"/>
+    <row r="125" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="47"/>
+      <c r="B125" s="41"/>
+      <c r="C125" s="45"/>
       <c r="D125" s="20"/>
-      <c r="E125" s="46"/>
+      <c r="E125" s="33"/>
       <c r="F125" s="17"/>
       <c r="G125" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A126" s="60"/>
-      <c r="B126" s="52"/>
-      <c r="C126" s="58"/>
+    <row r="126" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A126" s="47"/>
+      <c r="B126" s="39"/>
+      <c r="C126" s="45"/>
       <c r="D126" s="20"/>
-      <c r="E126" s="46"/>
+      <c r="E126" s="33"/>
       <c r="F126" s="18"/>
       <c r="G126" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="60"/>
-      <c r="B127" s="53"/>
-      <c r="C127" s="58"/>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="47"/>
+      <c r="B127" s="40"/>
+      <c r="C127" s="45"/>
       <c r="D127" s="20"/>
-      <c r="E127" s="46"/>
+      <c r="E127" s="33"/>
       <c r="F127" s="18"/>
       <c r="G127" s="14"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="61"/>
-      <c r="B128" s="54"/>
-      <c r="C128" s="58"/>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="48"/>
+      <c r="B128" s="41"/>
+      <c r="C128" s="45"/>
       <c r="D128" s="20"/>
-      <c r="E128" s="46"/>
+      <c r="E128" s="33"/>
       <c r="F128" s="18"/>
       <c r="G128" s="14"/>
     </row>
-    <row r="129" spans="1:7" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
-      <c r="C129" s="58"/>
+      <c r="C129" s="45"/>
       <c r="D129" s="20"/>
       <c r="E129" s="4"/>
       <c r="F129" s="3"/>
       <c r="G129" s="14"/>
     </row>
-    <row r="130" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="59"/>
-      <c r="B130" s="52"/>
-      <c r="C130" s="65"/>
+    <row r="130" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="46"/>
+      <c r="B130" s="39"/>
+      <c r="C130" s="52"/>
       <c r="D130" s="20"/>
-      <c r="E130" s="47"/>
+      <c r="E130" s="34"/>
       <c r="F130" s="14"/>
       <c r="G130" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="60"/>
-      <c r="B131" s="53"/>
-      <c r="C131" s="63"/>
+    <row r="131" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="47"/>
+      <c r="B131" s="40"/>
+      <c r="C131" s="50"/>
       <c r="D131" s="16"/>
-      <c r="E131" s="47"/>
+      <c r="E131" s="34"/>
       <c r="F131" s="14"/>
       <c r="G131" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A132" s="60"/>
-      <c r="B132" s="54"/>
+    <row r="132" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A132" s="47"/>
+      <c r="B132" s="41"/>
       <c r="C132" s="28"/>
       <c r="D132" s="20"/>
-      <c r="E132" s="47"/>
+      <c r="E132" s="34"/>
       <c r="F132" s="14"/>
       <c r="G132" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="60"/>
-      <c r="B133" s="52"/>
-      <c r="C133" s="58"/>
+    <row r="133" spans="1:7" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="47"/>
+      <c r="B133" s="39"/>
+      <c r="C133" s="45"/>
       <c r="D133" s="20"/>
-      <c r="E133" s="47"/>
+      <c r="E133" s="34"/>
       <c r="F133" s="14"/>
       <c r="G133" s="3"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="60"/>
-      <c r="B134" s="53"/>
-      <c r="C134" s="58"/>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="47"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="45"/>
       <c r="D134" s="20"/>
-      <c r="E134" s="47"/>
+      <c r="E134" s="34"/>
       <c r="F134" s="14"/>
       <c r="G134" s="14"/>
     </row>
-    <row r="135" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="60"/>
-      <c r="B135" s="54"/>
-      <c r="C135" s="58"/>
+    <row r="135" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="47"/>
+      <c r="B135" s="41"/>
+      <c r="C135" s="45"/>
       <c r="D135" s="20"/>
-      <c r="E135" s="47"/>
+      <c r="E135" s="34"/>
       <c r="F135" s="14"/>
       <c r="G135" s="14"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" s="60"/>
-      <c r="B136" s="52"/>
-      <c r="C136" s="58"/>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="47"/>
+      <c r="B136" s="39"/>
+      <c r="C136" s="45"/>
       <c r="D136" s="20"/>
-      <c r="E136" s="47"/>
+      <c r="E136" s="34"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
     </row>
-    <row r="137" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="60"/>
-      <c r="B137" s="53"/>
-      <c r="C137" s="58"/>
+    <row r="137" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="47"/>
+      <c r="B137" s="40"/>
+      <c r="C137" s="45"/>
       <c r="D137" s="20"/>
-      <c r="E137" s="47"/>
+      <c r="E137" s="34"/>
       <c r="F137" s="14"/>
       <c r="G137" s="14"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" s="60"/>
-      <c r="B138" s="54"/>
-      <c r="C138" s="58"/>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="47"/>
+      <c r="B138" s="41"/>
+      <c r="C138" s="45"/>
       <c r="D138" s="20"/>
-      <c r="E138" s="47"/>
+      <c r="E138" s="34"/>
       <c r="F138" s="14"/>
       <c r="G138" s="14"/>
     </row>
-    <row r="139" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="60"/>
-      <c r="B139" s="52"/>
-      <c r="C139" s="58"/>
+    <row r="139" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="47"/>
+      <c r="B139" s="39"/>
+      <c r="C139" s="45"/>
       <c r="D139" s="20"/>
-      <c r="E139" s="47"/>
+      <c r="E139" s="34"/>
       <c r="F139" s="14"/>
       <c r="G139" s="14"/>
     </row>
-    <row r="140" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="60"/>
-      <c r="B140" s="53"/>
-      <c r="C140" s="58"/>
+    <row r="140" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="47"/>
+      <c r="B140" s="40"/>
+      <c r="C140" s="45"/>
       <c r="D140" s="20"/>
-      <c r="E140" s="47"/>
+      <c r="E140" s="34"/>
       <c r="F140" s="14"/>
       <c r="G140" s="14"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="60"/>
-      <c r="B141" s="54"/>
-      <c r="C141" s="58"/>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="47"/>
+      <c r="B141" s="41"/>
+      <c r="C141" s="45"/>
       <c r="D141" s="20"/>
-      <c r="E141" s="47"/>
+      <c r="E141" s="34"/>
       <c r="F141" s="14"/>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="60"/>
-      <c r="B142" s="52"/>
-      <c r="C142" s="58"/>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="47"/>
+      <c r="B142" s="39"/>
+      <c r="C142" s="45"/>
       <c r="D142" s="20"/>
-      <c r="E142" s="47"/>
+      <c r="E142" s="34"/>
       <c r="F142" s="14"/>
       <c r="G142" s="14"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" s="60"/>
-      <c r="B143" s="53"/>
-      <c r="C143" s="58"/>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="47"/>
+      <c r="B143" s="40"/>
+      <c r="C143" s="45"/>
       <c r="D143" s="20"/>
-      <c r="E143" s="47"/>
+      <c r="E143" s="34"/>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" s="60"/>
-      <c r="B144" s="54"/>
-      <c r="C144" s="58"/>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="47"/>
+      <c r="B144" s="41"/>
+      <c r="C144" s="45"/>
       <c r="D144" s="20"/>
-      <c r="E144" s="47"/>
+      <c r="E144" s="34"/>
       <c r="F144" s="14"/>
       <c r="G144" s="14"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A145" s="60"/>
-      <c r="B145" s="52"/>
-      <c r="C145" s="58"/>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="47"/>
+      <c r="B145" s="39"/>
+      <c r="C145" s="45"/>
       <c r="D145" s="20"/>
-      <c r="E145" s="47"/>
+      <c r="E145" s="34"/>
       <c r="F145" s="14"/>
       <c r="G145" s="14"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="60"/>
-      <c r="B146" s="53"/>
-      <c r="C146" s="58"/>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="47"/>
+      <c r="B146" s="40"/>
+      <c r="C146" s="45"/>
       <c r="D146" s="20"/>
-      <c r="E146" s="47"/>
+      <c r="E146" s="34"/>
       <c r="F146" s="14"/>
       <c r="G146" s="14"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="60"/>
-      <c r="B147" s="54"/>
-      <c r="C147" s="58"/>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="47"/>
+      <c r="B147" s="41"/>
+      <c r="C147" s="45"/>
       <c r="D147" s="20"/>
-      <c r="E147" s="47"/>
+      <c r="E147" s="34"/>
       <c r="F147" s="14"/>
       <c r="G147" s="14"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="60"/>
-      <c r="B148" s="52"/>
-      <c r="C148" s="58"/>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="47"/>
+      <c r="B148" s="39"/>
+      <c r="C148" s="45"/>
       <c r="D148" s="20"/>
-      <c r="E148" s="47"/>
+      <c r="E148" s="34"/>
       <c r="F148" s="14"/>
       <c r="G148" s="14"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="60"/>
-      <c r="B149" s="53"/>
-      <c r="C149" s="58"/>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="47"/>
+      <c r="B149" s="40"/>
+      <c r="C149" s="45"/>
       <c r="D149" s="20"/>
-      <c r="E149" s="47"/>
+      <c r="E149" s="34"/>
       <c r="F149" s="14"/>
       <c r="G149" s="14"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="60"/>
-      <c r="B150" s="54"/>
-      <c r="C150" s="58"/>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="47"/>
+      <c r="B150" s="41"/>
+      <c r="C150" s="45"/>
       <c r="D150" s="20"/>
-      <c r="E150" s="47"/>
+      <c r="E150" s="34"/>
       <c r="F150" s="14"/>
       <c r="G150" s="14"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="60"/>
-      <c r="B151" s="52"/>
-      <c r="C151" s="58"/>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="47"/>
+      <c r="B151" s="39"/>
+      <c r="C151" s="45"/>
       <c r="D151" s="20"/>
-      <c r="E151" s="47"/>
+      <c r="E151" s="34"/>
       <c r="F151" s="14"/>
       <c r="G151" s="14"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="60"/>
-      <c r="B152" s="53"/>
-      <c r="C152" s="58"/>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="47"/>
+      <c r="B152" s="40"/>
+      <c r="C152" s="45"/>
       <c r="D152" s="20"/>
-      <c r="E152" s="47"/>
+      <c r="E152" s="34"/>
       <c r="F152" s="14"/>
       <c r="G152" s="14"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="60"/>
-      <c r="B153" s="54"/>
-      <c r="C153" s="58"/>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="47"/>
+      <c r="B153" s="41"/>
+      <c r="C153" s="45"/>
       <c r="D153" s="20"/>
-      <c r="E153" s="47"/>
+      <c r="E153" s="34"/>
       <c r="F153" s="14"/>
       <c r="G153" s="14"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C154" s="64"/>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C154" s="51"/>
       <c r="D154" s="20"/>
       <c r="G154" s="14"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C155" s="64"/>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C155" s="51"/>
       <c r="D155" s="20"/>
       <c r="G155" s="14"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C156" s="64"/>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C156" s="51"/>
       <c r="G156" s="14"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G157" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B31:B47"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="B83:B85"/>
     <mergeCell ref="B86:B88"/>
     <mergeCell ref="B22:B25"/>
@@ -4541,10 +4550,11 @@
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B31:B47"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B80:B82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B31:B33" location="'Product Backlog'!B11" display="RF009" xr:uid="{C3A8409B-FF61-A540-AA01-5A22BA3F613C}"/>
@@ -4567,55 +4577,55 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="62" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="36"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="54"/>
+      <c r="B2" s="63"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="46"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="37"/>
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="64"/>
       <c r="D3" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="46"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="35" t="s">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="18" t="s">
         <v>174</v>
       </c>
@@ -4623,13 +4633,13 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="36"/>
+    <row r="5" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="63"/>
       <c r="D5" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="18" t="s">
         <v>174</v>
       </c>
@@ -4637,121 +4647,121 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="37"/>
+    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="64"/>
       <c r="D6" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="46"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="46"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
+      <c r="B8" s="63"/>
       <c r="D8" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="E8" s="46"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="37"/>
+    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="54"/>
+      <c r="B9" s="64"/>
       <c r="D9" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="46"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="35" t="s">
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="54"/>
+      <c r="B10" s="62" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E10" s="46"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="B11" s="63"/>
       <c r="D11" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="46"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="37"/>
+    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="64"/>
       <c r="D12" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="35" t="s">
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="62" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="37"/>
+    <row r="14" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="55"/>
+      <c r="B14" s="64"/>
       <c r="D14" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="46"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="2.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="D15" s="20" t="s">
@@ -4761,297 +4771,297 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="62" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="46"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="36"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="63"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="46"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="36"/>
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="63"/>
       <c r="D18" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="46"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="37"/>
+    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+      <c r="B19" s="64"/>
       <c r="D19" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="46"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="35" t="s">
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="54"/>
+      <c r="B20" s="62" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="46"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="36"/>
+    <row r="21" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="54"/>
+      <c r="B21" s="63"/>
       <c r="D21" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="46"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="37"/>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="54"/>
+      <c r="B22" s="64"/>
       <c r="D22" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="E22" s="46"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="35" t="s">
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="54"/>
+      <c r="B23" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="46"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="36"/>
+    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="54"/>
+      <c r="B24" s="63"/>
       <c r="D24" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="E24" s="46"/>
+      <c r="E24" s="33"/>
       <c r="F24" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="B25" s="36"/>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+      <c r="B25" s="63"/>
       <c r="D25" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="E25" s="46"/>
+      <c r="E25" s="33"/>
       <c r="F25" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
-      <c r="B26" s="37"/>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
+      <c r="B26" s="64"/>
       <c r="D26" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="46"/>
+      <c r="E26" s="33"/>
       <c r="F26" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="35" t="s">
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="54"/>
+      <c r="B27" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E27" s="46"/>
+      <c r="E27" s="33"/>
       <c r="F27" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
-      <c r="B28" s="36"/>
+    <row r="28" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A28" s="54"/>
+      <c r="B28" s="63"/>
       <c r="D28" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="46"/>
+      <c r="E28" s="33"/>
       <c r="F28" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="30"/>
-      <c r="B29" s="37"/>
+    <row r="29" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
+      <c r="B29" s="64"/>
       <c r="D29" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="46"/>
+      <c r="E29" s="33"/>
       <c r="F29" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="35" t="s">
+    <row r="30" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+      <c r="B30" s="62" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="E30" s="46"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="30"/>
-      <c r="B31" s="36"/>
+    <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="63"/>
       <c r="D31" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="46"/>
+      <c r="E31" s="33"/>
       <c r="F31" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="30"/>
-      <c r="B32" s="37"/>
+    <row r="32" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="64"/>
       <c r="D32" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="46"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="35" t="s">
+    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
+      <c r="B33" s="62" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="E33" s="46"/>
+      <c r="E33" s="33"/>
       <c r="F33" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G33" s="14"/>
     </row>
-    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="36"/>
+    <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
+      <c r="B34" s="63"/>
       <c r="D34" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="46"/>
+      <c r="E34" s="33"/>
       <c r="F34" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G34" s="14"/>
     </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="37"/>
+    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
+      <c r="B35" s="64"/>
       <c r="D35" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="E35" s="46"/>
+      <c r="E35" s="33"/>
       <c r="F35" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="35" t="s">
+    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
+      <c r="B36" s="62" t="s">
         <v>66</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="E36" s="46"/>
+      <c r="E36" s="33"/>
       <c r="F36" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="36"/>
+    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="54"/>
+      <c r="B37" s="63"/>
       <c r="D37" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E37" s="46"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G37" s="14"/>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
-      <c r="B38" s="37"/>
+    <row r="38" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A38" s="55"/>
+      <c r="B38" s="64"/>
       <c r="D38" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="46"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" ht="2.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="D39" s="20" t="s">
@@ -5061,129 +5071,129 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="29" t="s">
+    <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="62" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="46"/>
+      <c r="E40" s="33"/>
       <c r="F40" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G40" s="14"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="36"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
+      <c r="B41" s="63"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="46"/>
+      <c r="E41" s="33"/>
       <c r="F41" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G41" s="14"/>
     </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="37"/>
+    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
+      <c r="B42" s="64"/>
       <c r="D42" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="E42" s="46"/>
+      <c r="E42" s="33"/>
       <c r="F42" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G42" s="14"/>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="30"/>
-      <c r="B43" s="35" t="s">
+    <row r="43" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A43" s="54"/>
+      <c r="B43" s="62" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="E43" s="46"/>
+      <c r="E43" s="33"/>
       <c r="F43" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G43" s="14"/>
     </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="36"/>
+    <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
+      <c r="B44" s="63"/>
       <c r="D44" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="E44" s="46"/>
+      <c r="E44" s="33"/>
       <c r="F44" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G44" s="14"/>
     </row>
-    <row r="45" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" s="30"/>
-      <c r="B45" s="37"/>
+    <row r="45" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="64"/>
       <c r="D45" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="E45" s="46"/>
+      <c r="E45" s="33"/>
       <c r="F45" s="19" t="s">
         <v>173</v>
       </c>
       <c r="G45" s="14"/>
     </row>
-    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="30"/>
-      <c r="B46" s="35" t="s">
+    <row r="46" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="62" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="46"/>
+      <c r="E46" s="33"/>
       <c r="F46" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G46" s="14"/>
     </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="30"/>
-      <c r="B47" s="36"/>
+    <row r="47" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
+      <c r="B47" s="63"/>
       <c r="D47" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E47" s="46"/>
+      <c r="E47" s="33"/>
       <c r="F47" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G47" s="14"/>
     </row>
-    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="30"/>
-      <c r="B48" s="37"/>
+    <row r="48" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="64"/>
       <c r="D48" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E48" s="46"/>
+      <c r="E48" s="33"/>
       <c r="F48" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A49" s="30"/>
-      <c r="B49" s="35" t="s">
+    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
+      <c r="B49" s="62" t="s">
         <v>7</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="E49" s="46"/>
+      <c r="E49" s="33"/>
       <c r="F49" s="18" t="s">
         <v>174</v>
       </c>
@@ -5191,13 +5201,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A50" s="30"/>
-      <c r="B50" s="36"/>
+    <row r="50" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="54"/>
+      <c r="B50" s="63"/>
       <c r="D50" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="E50" s="46"/>
+      <c r="E50" s="33"/>
       <c r="F50" s="18" t="s">
         <v>174</v>
       </c>
@@ -5205,13 +5215,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A51" s="30"/>
-      <c r="B51" s="37"/>
+    <row r="51" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A51" s="54"/>
+      <c r="B51" s="64"/>
       <c r="D51" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="E51" s="46"/>
+      <c r="E51" s="33"/>
       <c r="F51" s="18" t="s">
         <v>174</v>
       </c>
@@ -5219,53 +5229,53 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" s="30"/>
-      <c r="B52" s="35" t="s">
+    <row r="52" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A52" s="54"/>
+      <c r="B52" s="62" t="s">
         <v>44</v>
       </c>
       <c r="D52" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="E52" s="46"/>
+      <c r="E52" s="33"/>
       <c r="F52" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G52" s="14"/>
     </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
-      <c r="B53" s="36"/>
+    <row r="53" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" s="54"/>
+      <c r="B53" s="63"/>
       <c r="D53" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="E53" s="46"/>
+      <c r="E53" s="33"/>
       <c r="F53" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="30"/>
-      <c r="B54" s="37"/>
+    <row r="54" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A54" s="54"/>
+      <c r="B54" s="64"/>
       <c r="D54" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E54" s="46"/>
+      <c r="E54" s="33"/>
       <c r="F54" s="17" t="s">
         <v>172</v>
       </c>
       <c r="G54" s="14"/>
     </row>
-    <row r="55" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" s="30"/>
-      <c r="B55" s="35" t="s">
+    <row r="55" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A55" s="54"/>
+      <c r="B55" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E55" s="46"/>
+      <c r="E55" s="33"/>
       <c r="F55" s="18" t="s">
         <v>174</v>
       </c>
@@ -5273,13 +5283,13 @@
         <v>177</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A56" s="30"/>
-      <c r="B56" s="36"/>
+    <row r="56" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" s="54"/>
+      <c r="B56" s="63"/>
       <c r="D56" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="E56" s="46"/>
+      <c r="E56" s="33"/>
       <c r="F56" s="18" t="s">
         <v>174</v>
       </c>
@@ -5287,13 +5297,13 @@
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A57" s="31"/>
-      <c r="B57" s="37"/>
+    <row r="57" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="64"/>
       <c r="D57" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="E57" s="46"/>
+      <c r="E57" s="33"/>
       <c r="F57" s="18" t="s">
         <v>174</v>
       </c>
@@ -5301,7 +5311,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="D58" s="20" t="s">
@@ -5311,302 +5321,323 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="29" t="s">
+    <row r="59" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="62" t="s">
         <v>44</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="E59" s="47"/>
+      <c r="E59" s="34"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
     </row>
-    <row r="60" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30"/>
-      <c r="B60" s="36"/>
+    <row r="60" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="54"/>
+      <c r="B60" s="63"/>
       <c r="C60" s="28"/>
       <c r="D60" s="16"/>
-      <c r="E60" s="47"/>
+      <c r="E60" s="34"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
     </row>
-    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="30"/>
-      <c r="B61" s="37"/>
+    <row r="61" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A61" s="54"/>
+      <c r="B61" s="64"/>
       <c r="C61" s="28"/>
       <c r="D61" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="E61" s="47"/>
+      <c r="E61" s="34"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
     </row>
-    <row r="62" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
-      <c r="B62" s="35" t="s">
+    <row r="62" spans="1:7" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="54"/>
+      <c r="B62" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="38"/>
+      <c r="C62" s="65"/>
       <c r="D62" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E62" s="47"/>
+      <c r="E62" s="34"/>
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
     </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="30"/>
-      <c r="B63" s="36"/>
-      <c r="C63" s="38"/>
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="54"/>
+      <c r="B63" s="63"/>
+      <c r="C63" s="65"/>
       <c r="D63" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="E63" s="47"/>
+      <c r="E63" s="34"/>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
     </row>
-    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="30"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="38"/>
+    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="54"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="65"/>
       <c r="D64" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="47"/>
+      <c r="E64" s="34"/>
       <c r="F64" s="14"/>
       <c r="G64" s="14"/>
     </row>
-    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="30"/>
-      <c r="B65" s="35" t="s">
+    <row r="65" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="54"/>
+      <c r="B65" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="38"/>
+      <c r="C65" s="65"/>
       <c r="D65" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="E65" s="47"/>
+      <c r="E65" s="34"/>
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
     </row>
-    <row r="66" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="36"/>
-      <c r="C66" s="38"/>
+    <row r="66" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="54"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="65"/>
       <c r="D66" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="E66" s="47"/>
+      <c r="E66" s="34"/>
       <c r="F66" s="14"/>
       <c r="G66" s="14"/>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="30"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="38"/>
+    <row r="67" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="54"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="65"/>
       <c r="D67" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="E67" s="47"/>
+      <c r="E67" s="34"/>
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
     </row>
-    <row r="68" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="30"/>
-      <c r="B68" s="35" t="s">
+    <row r="68" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="54"/>
+      <c r="B68" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="38"/>
+      <c r="C68" s="65"/>
       <c r="D68" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E68" s="47"/>
+      <c r="E68" s="34"/>
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
     </row>
-    <row r="69" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="30"/>
-      <c r="B69" s="36"/>
-      <c r="C69" s="38"/>
+    <row r="69" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="54"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="65"/>
       <c r="D69" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="E69" s="47"/>
+      <c r="E69" s="34"/>
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
     </row>
-    <row r="70" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A70" s="30"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="38"/>
+    <row r="70" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A70" s="54"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="65"/>
       <c r="D70" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="E70" s="47"/>
+      <c r="E70" s="34"/>
       <c r="F70" s="14"/>
       <c r="G70" s="14"/>
     </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="30"/>
-      <c r="B71" s="35" t="s">
+    <row r="71" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A71" s="54"/>
+      <c r="B71" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="38"/>
+      <c r="C71" s="65"/>
       <c r="D71" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E71" s="47"/>
+      <c r="E71" s="34"/>
       <c r="F71" s="14"/>
       <c r="G71" s="14"/>
     </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="30"/>
-      <c r="B72" s="36"/>
-      <c r="C72" s="38"/>
+    <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="54"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="65"/>
       <c r="D72" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="E72" s="47"/>
+      <c r="E72" s="34"/>
       <c r="F72" s="14"/>
       <c r="G72" s="14"/>
     </row>
-    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="30"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="38"/>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="54"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="65"/>
       <c r="D73" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E73" s="47"/>
+      <c r="E73" s="34"/>
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
     </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="30"/>
-      <c r="B74" s="35" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="54"/>
+      <c r="B74" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C74" s="38"/>
+      <c r="C74" s="65"/>
       <c r="D74" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E74" s="47"/>
+      <c r="E74" s="34"/>
       <c r="F74" s="14"/>
       <c r="G74" s="14"/>
     </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="30"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="38"/>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="54"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="65"/>
       <c r="D75" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="E75" s="47"/>
+      <c r="E75" s="34"/>
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
     </row>
-    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="30"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="38"/>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="54"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="65"/>
       <c r="D76" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E76" s="47"/>
+      <c r="E76" s="34"/>
       <c r="F76" s="14"/>
       <c r="G76" s="14"/>
     </row>
-    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="30"/>
-      <c r="B77" s="35" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="54"/>
+      <c r="B77" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C77" s="38"/>
+      <c r="C77" s="65"/>
       <c r="D77" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E77" s="47"/>
+      <c r="E77" s="34"/>
       <c r="F77" s="14"/>
       <c r="G77" s="14"/>
     </row>
-    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="30"/>
-      <c r="B78" s="36"/>
-      <c r="C78" s="38"/>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="54"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="65"/>
       <c r="D78" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="E78" s="47"/>
+      <c r="E78" s="34"/>
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
     </row>
-    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="30"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="38"/>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="54"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="65"/>
       <c r="D79" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E79" s="47"/>
+      <c r="E79" s="34"/>
       <c r="F79" s="14"/>
       <c r="G79" s="14"/>
     </row>
-    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="30"/>
-      <c r="B80" s="35" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="54"/>
+      <c r="B80" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="38"/>
+      <c r="C80" s="65"/>
       <c r="D80" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E80" s="47"/>
+      <c r="E80" s="34"/>
       <c r="F80" s="14"/>
       <c r="G80" s="14"/>
     </row>
-    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="30"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="38"/>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="54"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="65"/>
       <c r="D81" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="E81" s="47"/>
+      <c r="E81" s="34"/>
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
     </row>
-    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="30"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="38"/>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="54"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E82" s="47"/>
+      <c r="E82" s="34"/>
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
     </row>
-    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D83" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E83" s="48"/>
-    </row>
-    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="E83" s="35"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D84" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="E84" s="48"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E85" s="48"/>
+      <c r="E84" s="35"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E85" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:A14"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A16:A38"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A40:A57"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B55:B57"/>
     <mergeCell ref="A59:A82"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="B62:B64"/>
@@ -5617,27 +5648,6 @@
     <mergeCell ref="B74:B76"/>
     <mergeCell ref="B77:B79"/>
     <mergeCell ref="B80:B82"/>
-    <mergeCell ref="A40:A57"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="A16:A38"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A1:A14"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>